<commit_message>
new plots and parity plots
</commit_message>
<xml_diff>
--- a/Domenique/paper plots (final)/data_final.xlsx
+++ b/Domenique/paper plots (final)/data_final.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Domenique\Desktop\TESCOR Project\Ammar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\Eclipse workspace\Trunk\Domenique\paper plots (final)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="345" windowWidth="19200" windowHeight="6953"/>
   </bookViews>
   <sheets>
-    <sheet name="T_dis" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -435,20 +435,20 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="20.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" customWidth="1"/>
-    <col min="6" max="6" width="18.1796875" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" customWidth="1"/>
-    <col min="8" max="8" width="19.6328125" customWidth="1"/>
-    <col min="9" max="9" width="18.7265625" customWidth="1"/>
-    <col min="10" max="10" width="16.6328125" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" customWidth="1"/>
+    <col min="5" max="5" width="19.19921875" customWidth="1"/>
+    <col min="6" max="6" width="18.19921875" customWidth="1"/>
+    <col min="7" max="7" width="19.265625" customWidth="1"/>
+    <col min="8" max="8" width="19.59765625" customWidth="1"/>
+    <col min="9" max="9" width="18.73046875" customWidth="1"/>
+    <col min="10" max="10" width="16.59765625" customWidth="1"/>
+    <col min="11" max="11" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -483,7 +483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>311.39999999999998</v>
       </c>
@@ -518,7 +518,7 @@
         <v>0.92710000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>310.39999999999998</v>
       </c>
@@ -553,7 +553,7 @@
         <v>0.89849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>316.89999999999998</v>
       </c>
@@ -588,7 +588,7 @@
         <v>0.90629999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>317.3</v>
       </c>
@@ -623,7 +623,7 @@
         <v>0.9173</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>322.39999999999998</v>
       </c>
@@ -658,7 +658,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>322.3</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.89180000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>322.3</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.88490000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>333.4</v>
       </c>
@@ -763,7 +763,7 @@
         <v>0.89670000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>326.8</v>
       </c>
@@ -798,7 +798,7 @@
         <v>0.8891</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>327.10000000000002</v>
       </c>
@@ -833,7 +833,7 @@
         <v>0.89529999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>327.7</v>
       </c>
@@ -868,7 +868,7 @@
         <v>0.9052</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>327.7</v>
       </c>
@@ -903,7 +903,7 @@
         <v>0.88549999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>327.7</v>
       </c>
@@ -938,7 +938,7 @@
         <v>0.89629999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>327.7</v>
       </c>
@@ -973,7 +973,7 @@
         <v>0.90769999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>316.7</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>316.60000000000002</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>0.92010000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>311.10000000000002</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>0.89529999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>311.10000000000002</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>0.9254</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>322.10000000000002</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>0.90749999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>322.2</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>0.88849999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>322.2</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>0.88329999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>333</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>0.89610000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>327.7</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>0.8921</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>327.60000000000002</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0.88460000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>327.60000000000002</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>0.90469999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>327.60000000000002</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>0.86060000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>311</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>0.89319999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>311.10000000000002</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0.89929999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>310.89999999999998</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>0.90800000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>311</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>0.9133</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>311.10000000000002</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>0.91820000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>310.7</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>322.2</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>0.90180000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>322.2</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>0.89590000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>322.39999999999998</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>0.8861</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>322</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0.88149999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>322.10000000000002</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0.87370000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>333.2</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0.89759999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>333.2</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>0.88890000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>316.60000000000002</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>0.91639999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>316.5</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>0.91010000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>316.5</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>0.90380000000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>322.2</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>0.90939999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C46" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new files and plots
</commit_message>
<xml_diff>
--- a/Domenique/paper plots (final)/data_final.xlsx
+++ b/Domenique/paper plots (final)/data_final.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1035" windowWidth="19200" windowHeight="6953"/>
+    <workbookView xWindow="0" yWindow="2070" windowWidth="19200" windowHeight="6953"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Injection Superheat (K)</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t>predicted heat loss (w/ T_amb)</t>
+  </si>
+  <si>
+    <t>PressureRatio</t>
+  </si>
+  <si>
+    <t>DELTAT_inj_sh</t>
+  </si>
+  <si>
+    <t>T_dis_ARI</t>
+  </si>
+  <si>
+    <t>f_loss_ARI</t>
+  </si>
+  <si>
+    <t>eta_v_ARI</t>
+  </si>
+  <si>
+    <t>m_ratio_ARI</t>
+  </si>
+  <si>
+    <t>eta_isen_ARI</t>
   </si>
 </sst>
 </file>
@@ -127,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -136,6 +157,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -452,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -469,9 +493,10 @@
     <col min="9" max="9" width="18.73046875" customWidth="1"/>
     <col min="10" max="10" width="16.59765625" customWidth="1"/>
     <col min="11" max="11" width="15.73046875" customWidth="1"/>
+    <col min="21" max="21" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -514,8 +539,29 @@
       <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>311.39999999999998</v>
       </c>
@@ -558,8 +604,34 @@
       <c r="N2">
         <v>3.3851203680170197</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O2">
+        <v>2.74</v>
+      </c>
+      <c r="P2">
+        <v>-0.26889999999999997</v>
+      </c>
+      <c r="Q2">
+        <f>665.0593909+0.817927021453*A2+0.00276112742963*A2^2+0.0000229182346928*A2^3-1.62264374721*B2-0.00383816931629*B2^2+0.0000537251962303*B2^3-0.008868928794*A2*B2-0.00002136670232*A2*B2^2-0.00002448785401*A2^2*B2</f>
+        <v>344.03348374734901</v>
+      </c>
+      <c r="R2">
+        <f>-4.465889875+0.0107360909672*A2+0.0000343103203327*A2^2-0.000000132222315321*A2^3-0.00143325862022*B2+0.00000345598124464*B2^2-0.000000113727106917*B2^3+0.0000430278967*A2*B2+0.00000002279244482*A2*B2^2+0.000000006045795432*A2^2*B2</f>
+        <v>7.5756316107959104E-2</v>
+      </c>
+      <c r="S2">
+        <f>169.0629066+0.469381128435*A2+0.00083348547161*A2^2-0.00000110098256054*A2^3-1.0042018431*B2-0.00318397009943*B2^2+0.0000134406588485*B2^3-0.001544169475*A2*B2+0.000002503405378*A2*B2^2-0.000001832161488*A2^2*B2</f>
+        <v>3.4843927919093929</v>
+      </c>
+      <c r="T2">
+        <f>-1.552608346+0.00220116615728*A2+0.00000454706451202*A2^2-0.0000000665161658137*A2^3+0.00421577359357*B2+0.0000121895400743*B2^2-0.000000108462358524*B2^3+0.00002487972751*A2*B2+0.00000002856676134*A2*B2^2+0.00000002716855885*A2^2*B2</f>
+        <v>0.92229918164685498</v>
+      </c>
+      <c r="U2">
+        <f>-3.511786579+0.00575172002971*A2+0.0000000498536022069*A2^2-0.000000271610183794*A2^3+0.00382867611365*B2-0.00000796961415441*B2^2-0.000000412819827189*B2^3+0.00008153326887*A2*B2+0.0000002621820947*A2*B2^2+0.0000002075530199*A2^2*B2</f>
+        <v>0.62625064105237183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>310.39999999999998</v>
       </c>
@@ -602,8 +674,34 @@
       <c r="N3">
         <v>3.0553871450680212</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O3">
+        <v>4.3789999999999996</v>
+      </c>
+      <c r="P3">
+        <v>-0.2021</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q44" si="0">665.0593909+0.817927021453*A3+0.00276112742963*A3^2+0.0000229182346928*A3^3-1.62264374721*B3-0.00383816931629*B3^2+0.0000537251962303*B3^3-0.008868928794*A3*B3-0.00002136670232*A3*B3^2-0.00002448785401*A3^2*B3</f>
+        <v>351.35094071368405</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R44" si="1">-4.465889875+0.0107360909672*A3+0.0000343103203327*A3^2-0.000000132222315321*A3^3-0.00143325862022*B3+0.00000345598124464*B3^2-0.000000113727106917*B3^3+0.0000430278967*A3*B3+0.00000002279244482*A3*B3^2+0.000000006045795432*A3^2*B3</f>
+        <v>0.16191477912422683</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S44" si="2">169.0629066+0.469381128435*A3+0.00083348547161*A3^2-0.00000110098256054*A3^3-1.0042018431*B3-0.00318397009943*B3^2+0.0000134406588485*B3^3-0.001544169475*A3*B3+0.000002503405378*A3*B3^2-0.000001832161488*A3^2*B3</f>
+        <v>3.4641360825831882</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T44" si="3">-1.552608346+0.00220116615728*A3+0.00000454706451202*A3^2-0.0000000665161658137*A3^3+0.00421577359357*B3+0.0000121895400743*B3^2-0.000000108462358524*B3^3+0.00002487972751*A3*B3+0.00000002856676134*A3*B3^2+0.00000002716855885*A3^2*B3</f>
+        <v>0.89356062904813038</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U44" si="4">-3.511786579+0.00575172002971*A3+0.0000000498536022069*A3^2-0.000000271610183794*A3^3+0.00382867611365*B3-0.00000796961415441*B3^2-0.000000412819827189*B3^3+0.00008153326887*A3*B3+0.0000002621820947*A3*B3^2+0.0000002075530199*A3^2*B3</f>
+        <v>0.64721025622365147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>316.89999999999998</v>
       </c>
@@ -646,8 +744,34 @@
       <c r="N4">
         <v>3.9012459879117705</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O4">
+        <v>3.8250000000000002</v>
+      </c>
+      <c r="P4">
+        <v>-0.2472</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>352.3380294636728</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>0.15902047853946991</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="2"/>
+        <v>3.788683925336727</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="3"/>
+        <v>0.90725341013657868</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="4"/>
+        <v>0.66066151703325193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>317.3</v>
       </c>
@@ -690,8 +814,34 @@
       <c r="N5">
         <v>4.0533568675775076</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O5">
+        <v>3.218</v>
+      </c>
+      <c r="P5">
+        <v>-0.2591</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>349.82408229203884</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>0.12445107915973813</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
+        <v>4.1111201339384991</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>0.91708355183565926</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="4"/>
+        <v>0.65288881098799845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>322.39999999999998</v>
       </c>
@@ -734,8 +884,34 @@
       <c r="N6">
         <v>4.6436302778637089</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O6">
+        <v>3.6190000000000002</v>
+      </c>
+      <c r="P6">
+        <v>-0.21859999999999999</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>355.61314695696569</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>0.15730029056660816</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>4.6688558958054998</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>0.91058673289664893</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="4"/>
+        <v>0.66295145954568113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>322.3</v>
       </c>
@@ -778,8 +954,34 @@
       <c r="N7">
         <v>4.2110119808190927</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O7">
+        <v>4.8079999999999998</v>
+      </c>
+      <c r="P7">
+        <v>-0.2</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>362.27263511081946</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>0.2105168547789327</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>4.4486545902435637</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>0.89102327384586621</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="4"/>
+        <v>0.65602563920811985</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>322.3</v>
       </c>
@@ -822,8 +1024,34 @@
       <c r="N8">
         <v>4.0853446528168034</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O8">
+        <v>5.3230000000000004</v>
+      </c>
+      <c r="P8">
+        <v>-0.22789999999999999</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>365.60567486487389</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0.22638961372272212</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>4.6405864592382073</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>0.88222760880532214</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="4"/>
+        <v>0.64570802761638735</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>333.4</v>
       </c>
@@ -866,8 +1094,34 @@
       <c r="N9">
         <v>6.002920710189918</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O9">
+        <v>4.3040000000000003</v>
+      </c>
+      <c r="P9">
+        <v>-0.2303</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>369.15699306190129</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>0.19750378148800632</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>5.9735112069479115</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>0.89268379510461304</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="4"/>
+        <v>0.655510512416698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>326.8</v>
       </c>
@@ -910,8 +1164,34 @@
       <c r="N10">
         <v>4.8609126641774552</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O10">
+        <v>4.8929999999999998</v>
+      </c>
+      <c r="P10">
+        <v>-0.15090000000000001</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>366.53156249436574</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>0.22023248203938217</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>4.8578844889568273</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="3"/>
+        <v>0.88843521990563357</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="4"/>
+        <v>0.65393722127167919</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>327.10000000000002</v>
       </c>
@@ -954,8 +1234,34 @@
       <c r="N11">
         <v>5.0013362713269744</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O11">
+        <v>4.4720000000000004</v>
+      </c>
+      <c r="P11">
+        <v>-0.22770000000000001</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>364.19031561659335</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>0.20426321576747905</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>4.9360787325097562</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>0.89526353982150775</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="4"/>
+        <v>0.66042455320269511</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>327.7</v>
       </c>
@@ -998,8 +1304,34 @@
       <c r="N12">
         <v>5.5827617511799099</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O12">
+        <v>3.7519999999999998</v>
+      </c>
+      <c r="P12">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>360.91481357390626</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>0.16866068096454928</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>5.4971387636383113</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>0.90597697008514888</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="4"/>
+        <v>0.66270185583703167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>327.7</v>
       </c>
@@ -1042,8 +1374,34 @@
       <c r="N13">
         <v>5.3504941208042922</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O13">
+        <v>4.9859999999999998</v>
+      </c>
+      <c r="P13">
+        <v>5.79</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>367.88821641752043</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>0.22429754484002937</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>4.9472433648542662</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="3"/>
+        <v>0.8865041382624238</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="4"/>
+        <v>0.6516643206960584</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>327.7</v>
       </c>
@@ -1086,8 +1444,34 @@
       <c r="N14">
         <v>5.8574436254020501</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O14">
+        <v>4.5490000000000004</v>
+      </c>
+      <c r="P14">
+        <v>5.5830000000000002</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>365.20556470052134</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>0.20810191824274341</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>4.9896981766209407</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="3"/>
+        <v>0.89361481118059427</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="4"/>
+        <v>0.65902931708458912</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>327.7</v>
       </c>
@@ -1130,8 +1514,34 @@
       <c r="N15">
         <v>6.2108962806940395</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O15">
+        <v>3.7559999999999998</v>
+      </c>
+      <c r="P15">
+        <v>5.82</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>360.91481357390626</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>0.16866068096454928</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>5.4971387636383113</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
+        <v>0.90597697008514888</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="4"/>
+        <v>0.66270185583703167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>316.7</v>
       </c>
@@ -1174,8 +1584,34 @@
       <c r="N16">
         <v>4.5614305330832616</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O16">
+        <v>3.806</v>
+      </c>
+      <c r="P16">
+        <v>5.7809999999999997</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>352.08787090565261</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>0.15759998992882154</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>3.7656246067232573</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="3"/>
+        <v>0.90752865175331954</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="4"/>
+        <v>0.660384616023868</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>316.60000000000002</v>
       </c>
@@ -1218,8 +1654,34 @@
       <c r="N17">
         <v>4.5627282817517107</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O17">
+        <v>3.1320000000000001</v>
+      </c>
+      <c r="P17">
+        <v>5.7469999999999999</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>348.97239736233905</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>0.11700897025996787</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>4.0660866613704911</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="3"/>
+        <v>0.91830432344326174</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="4"/>
+        <v>0.6496457207876869</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>311.10000000000002</v>
       </c>
@@ -1262,8 +1724,34 @@
       <c r="N18">
         <v>3.4047906991904417</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O18">
+        <v>4.431</v>
+      </c>
+      <c r="P18">
+        <v>5.8650000000000002</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>352.07106637570246</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>0.16616204768710321</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>3.5339361139878847</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>0.89330460025953395</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="4"/>
+        <v>0.64820160446395292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>311.10000000000002</v>
       </c>
@@ -1306,8 +1794,34 @@
       <c r="N19">
         <v>3.4291811887565524</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O19">
+        <v>2.72</v>
+      </c>
+      <c r="P19">
+        <v>5.673</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>343.79232861380444</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>7.4021563606017471E-2</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>3.438573208110121</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>0.92232601270087755</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="4"/>
+        <v>0.62510759427523244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>322.10000000000002</v>
       </c>
@@ -1350,8 +1864,34 @@
       <c r="N20">
         <v>4.7713857985735215</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O20">
+        <v>3.5870000000000002</v>
+      </c>
+      <c r="P20">
+        <v>5.7160000000000002</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>355.23998042550579</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="1"/>
+        <v>0.15536655464636959</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>4.6388883859686416</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>0.91107144952211461</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="4"/>
+        <v>0.66259877109257381</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>322.2</v>
       </c>
@@ -1394,8 +1934,34 @@
       <c r="N21">
         <v>4.5032509924111084</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O21">
+        <v>4.8049999999999997</v>
+      </c>
+      <c r="P21">
+        <v>5.4550000000000001</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>362.22833013850391</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="1"/>
+        <v>0.21051027774809039</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>4.4421134770915032</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>0.89093668536080506</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="4"/>
+        <v>0.65590647447472605</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>322.2</v>
       </c>
@@ -1438,8 +2004,34 @@
       <c r="N22">
         <v>4.2832282790452396</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O22">
+        <v>5.3140000000000001</v>
+      </c>
+      <c r="P22">
+        <v>5.7370000000000001</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="0"/>
+        <v>365.44137434509923</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="1"/>
+        <v>0.22581030069889613</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="2"/>
+        <v>4.6290989290578182</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>0.88245291665019687</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="4"/>
+        <v>0.64598430069026946</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>333</v>
       </c>
@@ -1482,8 +2074,34 @@
       <c r="N23">
         <v>6.3261085857665602</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O23">
+        <v>4.242</v>
+      </c>
+      <c r="P23">
+        <v>5.7859999999999996</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="0"/>
+        <v>368.46385689924819</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="1"/>
+        <v>0.19497297619464674</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="2"/>
+        <v>5.95505679138396</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="3"/>
+        <v>0.89393902565725325</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="4"/>
+        <v>0.6565674112912081</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>327.7</v>
       </c>
@@ -1526,8 +2144,34 @@
       <c r="N24">
         <v>5.094354754980837</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O24">
+        <v>4.4740000000000002</v>
+      </c>
+      <c r="P24">
+        <v>26.49</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="0"/>
+        <v>364.74134433590973</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>0.20485935592770332</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="2"/>
+        <v>5.0113299704008654</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="3"/>
+        <v>0.89487740979928654</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="4"/>
+        <v>0.66004031540120867</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>327.60000000000002</v>
       </c>
@@ -1570,8 +2214,34 @@
       <c r="N25">
         <v>5.434697094111149</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O25">
+        <v>4.931</v>
+      </c>
+      <c r="P25">
+        <v>28.41</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>367.3925550961834</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="1"/>
+        <v>0.22197230501403195</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="2"/>
+        <v>4.9362810566107314</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="3"/>
+        <v>0.88761997308609542</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="4"/>
+        <v>0.65298800469187057</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>327.60000000000002</v>
       </c>
@@ -1614,8 +2284,34 @@
       <c r="N26">
         <v>4.8659241367620547</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O26">
+        <v>3.7120000000000002</v>
+      </c>
+      <c r="P26">
+        <v>21.69</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>360.617595368563</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="1"/>
+        <v>0.16587058288515388</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="2"/>
+        <v>5.5310563688195558</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="3"/>
+        <v>0.90670353389210789</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="4"/>
+        <v>0.66240743188662066</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>327.60000000000002</v>
       </c>
@@ -1658,8 +2354,34 @@
       <c r="N27">
         <v>5.8962557523441443</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O27">
+        <v>6.7160000000000002</v>
+      </c>
+      <c r="P27">
+        <v>34.020000000000003</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="0"/>
+        <v>379.05340589428306</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="1"/>
+        <v>0.26771250904544275</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="2"/>
+        <v>5.558280595009478</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="3"/>
+        <v>0.85849493383816111</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="4"/>
+        <v>0.60628837275779102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>311</v>
       </c>
@@ -1702,8 +2424,34 @@
       <c r="N28">
         <v>3.518451217797478</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O28">
+        <v>4.431</v>
+      </c>
+      <c r="P28">
+        <v>22.64</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>352.04296155560041</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="1"/>
+        <v>0.16596478516363128</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="2"/>
+        <v>3.5327370588461378</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="3"/>
+        <v>0.89312651843571012</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="4"/>
+        <v>0.64793703466689401</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>311.10000000000002</v>
       </c>
@@ -1746,8 +2494,34 @@
       <c r="N29">
         <v>3.5806778445208978</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O29">
+        <v>3.972</v>
+      </c>
+      <c r="P29">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="0"/>
+        <v>349.37033035559011</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>0.14965319016323445</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="2"/>
+        <v>3.2584640724362686</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="3"/>
+        <v>0.9012937113064079</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="4"/>
+        <v>0.65131323548630515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>310.89999999999998</v>
       </c>
@@ -1790,8 +2564,34 @@
       <c r="N30">
         <v>3.1745903824421391</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O30">
+        <v>3.6040000000000001</v>
+      </c>
+      <c r="P30">
+        <v>18.38</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>347.09047919327759</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="1"/>
+        <v>0.13159989678624276</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="2"/>
+        <v>3.0944985640414089</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>0.90797806848854834</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="4"/>
+        <v>0.65004917664076611</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>311</v>
       </c>
@@ -1834,8 +2634,34 @@
       <c r="N31">
         <v>3.1824118159624764</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O31">
+        <v>3.2709999999999999</v>
+      </c>
+      <c r="P31">
+        <v>15.55</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="0"/>
+        <v>345.50338705997206</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>0.11342522114867221</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="2"/>
+        <v>3.0862797460643137</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="3"/>
+        <v>0.91385671664603163</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="4"/>
+        <v>0.64552332112265809</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>311.10000000000002</v>
       </c>
@@ -1878,8 +2704,34 @@
       <c r="N32">
         <v>3.2529731133638879</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O32">
+        <v>2.9670000000000001</v>
+      </c>
+      <c r="P32">
+        <v>12.79</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>344.38752692671858</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="1"/>
+        <v>9.3243927124110865E-2</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="2"/>
+        <v>3.2182349993256878</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="3"/>
+        <v>0.91886444546324775</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="4"/>
+        <v>0.6366664601430907</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>310.7</v>
       </c>
@@ -1922,8 +2774,34 @@
       <c r="N33">
         <v>3.1214903697604988</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O33">
+        <v>2.6829999999999998</v>
+      </c>
+      <c r="P33">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="0"/>
+        <v>343.44079842623887</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>6.9839106183753941E-2</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="2"/>
+        <v>3.4031605117773225</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="3"/>
+        <v>0.92262901811053577</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="4"/>
+        <v>0.62228656527669646</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>322.2</v>
       </c>
@@ -1966,8 +2844,34 @@
       <c r="N34">
         <v>4.3514370784605587</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O34">
+        <v>3.927</v>
+      </c>
+      <c r="P34">
+        <v>22.62</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="0"/>
+        <v>356.94646640945257</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>0.17362723400230223</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="2"/>
+        <v>4.4608237830307829</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="3"/>
+        <v>0.90587761059381533</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="4"/>
+        <v>0.66448090095170897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>322.2</v>
       </c>
@@ -2010,8 +2914,34 @@
       <c r="N35">
         <v>4.1467335814912865</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O35">
+        <v>4.3520000000000003</v>
+      </c>
+      <c r="P35">
+        <v>25.53</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="0"/>
+        <v>359.39991904638839</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="1"/>
+        <v>0.19339424821183659</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="2"/>
+        <v>4.3788979975885383</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="3"/>
+        <v>0.89871401157058128</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="4"/>
+        <v>0.6622356133099121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>322.39999999999998</v>
       </c>
@@ -2054,8 +2984,34 @@
       <c r="N36">
         <v>4.7343416932219391</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O36">
+        <v>4.8150000000000004</v>
+      </c>
+      <c r="P36">
+        <v>26.47</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="0"/>
+        <v>362.42719176701485</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="1"/>
+        <v>0.2111108904826853</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="2"/>
+        <v>4.4597404759369681</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="3"/>
+        <v>0.89081307515231334</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="4"/>
+        <v>0.65584488074858083</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>322</v>
       </c>
@@ -2098,8 +3054,34 @@
       <c r="N37">
         <v>4.3241934840249643</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O37">
+        <v>5.327</v>
+      </c>
+      <c r="P37">
+        <v>31.22</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="0"/>
+        <v>365.3692283989285</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="1"/>
+        <v>0.22573518344974947</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="2"/>
+        <v>4.6247537604767999</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="3"/>
+        <v>0.88223617815089761</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="4"/>
+        <v>0.64565584819172361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>322.10000000000002</v>
       </c>
@@ -2142,8 +3124,34 @@
       <c r="N38">
         <v>4.5339767672504392</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O38">
+        <v>5.9240000000000004</v>
+      </c>
+      <c r="P38">
+        <v>31.41</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="0"/>
+        <v>369.24183109625551</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="1"/>
+        <v>0.24037765158548133</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="2"/>
+        <v>4.9540189076543868</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="3"/>
+        <v>0.87252013246883819</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="4"/>
+        <v>0.63158180601436786</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>333.2</v>
       </c>
@@ -2186,8 +3194,34 @@
       <c r="N39">
         <v>4.7267179776448325</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O39">
+        <v>4.2859999999999996</v>
+      </c>
+      <c r="P39">
+        <v>28.75</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="0"/>
+        <v>368.84724590797202</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="1"/>
+        <v>0.19659675160353857</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="2"/>
+        <v>5.9576490414399927</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="3"/>
+        <v>0.89320958839315168</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="4"/>
+        <v>0.65599581313907507</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>333.2</v>
       </c>
@@ -2230,8 +3264,34 @@
       <c r="N40">
         <v>5.5130927827618148</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O40">
+        <v>4.702</v>
+      </c>
+      <c r="P40">
+        <v>30.23</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="0"/>
+        <v>371.24909894012194</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="1"/>
+        <v>0.21573183544176053</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="2"/>
+        <v>5.6575680875356369</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="3"/>
+        <v>0.88679035746836921</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="4"/>
+        <v>0.65072927383541135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>316.60000000000002</v>
       </c>
@@ -2274,8 +3334,34 @@
       <c r="N41">
         <v>3.7181407158166766</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O41">
+        <v>3.1030000000000002</v>
+      </c>
+      <c r="P41">
+        <v>14.28</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="0"/>
+        <v>348.90486236959123</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="1"/>
+        <v>0.11548793950800648</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="2"/>
+        <v>4.0873607765740729</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="3"/>
+        <v>0.91860480175741177</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="4"/>
+        <v>0.64895803110051276</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>316.5</v>
       </c>
@@ -2318,8 +3404,34 @@
       <c r="N42">
         <v>3.9263246519769859</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O42">
+        <v>3.4239999999999999</v>
+      </c>
+      <c r="P42">
+        <v>16.7</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="0"/>
+        <v>350.03677862902862</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="1"/>
+        <v>0.13615488064955439</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="2"/>
+        <v>3.8363959430136347</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="3"/>
+        <v>0.91382705361986849</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="4"/>
+        <v>0.65658038392398144</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>316.5</v>
       </c>
@@ -2362,8 +3474,34 @@
       <c r="N43">
         <v>3.9397534967994656</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O43">
+        <v>3.766</v>
+      </c>
+      <c r="P43">
+        <v>19.16</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="0"/>
+        <v>351.69679350714694</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="1"/>
+        <v>0.15483637402744516</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="2"/>
+        <v>3.7443277217488884</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="3"/>
+        <v>0.90825199323480066</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="4"/>
+        <v>0.65999159707223409</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>322.2</v>
       </c>
@@ -2406,8 +3544,34 @@
       <c r="N44">
         <v>4.1568334085298284</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="O44">
+        <v>3.5680000000000001</v>
+      </c>
+      <c r="P44">
+        <v>19.96</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="0"/>
+        <v>355.20260272175949</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="1"/>
+        <v>0.15382895343143027</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="2"/>
+        <v>4.678844571536608</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="3"/>
+        <v>0.91145718760723671</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="4"/>
+        <v>0.66228530964619292</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.45">
       <c r="C46" s="1"/>
     </row>
   </sheetData>

</xml_diff>